<commit_message>
Executing perfectly using Maven commands
</commit_message>
<xml_diff>
--- a/Sept9_TestNGPageObjModel/Test_IP_OP/ModuleDriver.xlsx
+++ b/Sept9_TestNGPageObjModel/Test_IP_OP/ModuleDriver.xlsx
@@ -390,7 +390,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -429,7 +429,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>